<commit_message>
Update Template excel and Add new employee function
</commit_message>
<xml_diff>
--- a/Base.API/wwwroot/template_schedule.xlsx
+++ b/Base.API/wwwroot/template_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FPT\Study\Summer 2024_DoAn\SEP490\materials\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Dropbox\PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FD710F-032C-411A-A2F3-301987A74951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5B62D0-CE73-453A-AA7F-5025CD29DBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>MON</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>2. Nếu không có dữ liệu, vui lòng để trống hoặc thay bằng dấu '-'</t>
-  </si>
-  <si>
-    <t>(Attended)</t>
   </si>
   <si>
     <t>Sample: 
@@ -148,28 +145,28 @@
  - SE1824-PRJ301 at NVH.222</t>
   </si>
   <si>
-    <t>22/07</t>
-  </si>
-  <si>
-    <t>23/07</t>
-  </si>
-  <si>
-    <t>24/07</t>
-  </si>
-  <si>
-    <t>25/07</t>
-  </si>
-  <si>
-    <t>26/07</t>
-  </si>
-  <si>
-    <t>27/07</t>
-  </si>
-  <si>
-    <t>28/07</t>
-  </si>
-  <si>
-    <t>SU24SE025_GSU35 at P.005</t>
+    <t>SE1824-IoT102t at P.005</t>
+  </si>
+  <si>
+    <t>05/08</t>
+  </si>
+  <si>
+    <t>06/08</t>
+  </si>
+  <si>
+    <t>07/08</t>
+  </si>
+  <si>
+    <t>08/08</t>
+  </si>
+  <si>
+    <t>09/08</t>
+  </si>
+  <si>
+    <t>10/08</t>
+  </si>
+  <si>
+    <t>11/08</t>
   </si>
 </sst>
 </file>
@@ -351,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -440,6 +437,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,7 +782,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -814,29 +814,29 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -945,15 +945,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
+    <col min="6" max="8" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -961,7 +963,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -976,13 +978,15 @@
       <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="18"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -996,10 +1000,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1016,10 +1020,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="18"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1035,8 +1039,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
+      <c r="A5" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1054,7 +1058,9 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1072,7 +1078,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1090,7 +1096,9 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1107,11 +1115,9 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="19"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
@@ -1131,9 +1137,7 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1177,9 +1181,7 @@
       <c r="R12" s="12"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1201,9 +1203,7 @@
       <c r="R13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1268,7 +1268,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="1"/>
       <c r="J17" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>

</xml_diff>